<commit_message>
agregando pacientes con cita a excel y error en la recuperacion de excel
</commit_message>
<xml_diff>
--- a/src/general/pacientes.xlsx
+++ b/src/general/pacientes.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <workbookPr/>
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nick paredes\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luigg\Desktop\ProyectoADA-Clinica\src\general\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1228D590-8A2F-419E-A913-4F524CAD5597}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20400" windowHeight="7035"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="10">
   <si>
     <t>nick</t>
   </si>
@@ -36,14 +37,41 @@
   </si>
   <si>
     <t>vacunado</t>
+  </si>
+  <si>
+    <t>codigo</t>
+  </si>
+  <si>
+    <t>LUIGGI</t>
+  </si>
+  <si>
+    <t>PASACHE LOPERA</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>ASDASD</t>
+  </si>
+  <si>
+    <t>ASDASDASD ADSASDASD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -71,8 +99,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -352,14 +381,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G17" sqref="A12:G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.85546875" collapsed="true"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -581,18 +614,18 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C12" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="D12" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
         <v>2</v>
@@ -601,47 +634,28 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>1</v>
-      </c>
-      <c r="D14" t="s">
-        <v>0</v>
-      </c>
-      <c r="E14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
agregando nuevo algoritmo para recomendacion de clinicas
</commit_message>
<xml_diff>
--- a/src/general/pacientes.xlsx
+++ b/src/general/pacientes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="14">
   <si>
     <t>nick</t>
   </si>
@@ -55,6 +55,18 @@
   </si>
   <si>
     <t>ASDASDASD ADSASDASD</t>
+  </si>
+  <si>
+    <t>ASDA</t>
+  </si>
+  <si>
+    <t>ASDAD ASDASD</t>
+  </si>
+  <si>
+    <t>LUIGGI STEEP</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -639,16 +651,16 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="F13" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
mejorando algoritmo de ordenamiento en hashtableclinica por quicksort
</commit_message>
<xml_diff>
--- a/src/general/pacientes.xlsx
+++ b/src/general/pacientes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="16">
   <si>
     <t>nick</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>F</t>
+  </si>
+  <si>
+    <t>WASD WASD</t>
+  </si>
+  <si>
+    <t>ASD ASDASD</t>
   </si>
 </sst>
 </file>
@@ -651,10 +657,10 @@
         <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
creando paquete util, quitanto imports innecesarios modificando metodos de crear citas
</commit_message>
<xml_diff>
--- a/src/general/pacientes.xlsx
+++ b/src/general/pacientes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="25">
   <si>
     <t>nick</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>ASD ASDASD</t>
+  </si>
+  <si>
+    <t>11236489</t>
   </si>
 </sst>
 </file>
@@ -678,7 +681,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
         <v>22</v>

</xml_diff>

<commit_message>
correccion cola de prioridad
</commit_message>
<xml_diff>
--- a/src/general/pacientes.xlsx
+++ b/src/general/pacientes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="42">
   <si>
     <t>nick</t>
   </si>
@@ -127,6 +127,30 @@
   </si>
   <si>
     <t>52</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>11236480</t>
+  </si>
+  <si>
+    <t>11236487</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>70</t>
   </si>
 </sst>
 </file>
@@ -717,7 +741,7 @@
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Revert "correccion cola de prioridad"
This reverts commit 726e2f03b85b65654b3378c7967357ec6dd6808a.
</commit_message>
<xml_diff>
--- a/src/general/pacientes.xlsx
+++ b/src/general/pacientes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="34">
   <si>
     <t>nick</t>
   </si>
@@ -127,30 +127,6 @@
   </si>
   <si>
     <t>52</t>
-  </si>
-  <si>
-    <t>60</t>
-  </si>
-  <si>
-    <t>11236480</t>
-  </si>
-  <si>
-    <t>11236487</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>32</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>70</t>
   </si>
 </sst>
 </file>
@@ -741,7 +717,7 @@
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Revert "Revert "correccion cola de prioridad""
This reverts commit 22523ef6865c54d4757dcddd83572e12155860bf.
</commit_message>
<xml_diff>
--- a/src/general/pacientes.xlsx
+++ b/src/general/pacientes.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="42">
   <si>
     <t>nick</t>
   </si>
@@ -127,6 +127,30 @@
   </si>
   <si>
     <t>52</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>11236480</t>
+  </si>
+  <si>
+    <t>11236487</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>32</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>70</t>
   </si>
 </sst>
 </file>
@@ -717,7 +741,7 @@
         <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="E13" t="s">
         <v>12</v>

</xml_diff>